<commit_message>
Operation Chaining 8ns vivado report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/OperationChaining8nsSolution/power/OperationChaining8nsDSPPowerReport.xlsx
+++ b/reports/vivado/OperationChaining8nsSolution/power/OperationChaining8nsDSPPowerReport.xlsx
@@ -172,7 +172,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>3.636262263171375E-4</v>
+        <v>3.64705512765795E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -198,7 +198,7 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>2.006586000788957E-4</v>
+        <v>2.0177781698293984E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
@@ -219,12 +219,12 @@
         <v>13</v>
       </c>
       <c r="H3" t="n" s="2">
-        <v>5.358490943908691</v>
+        <v>5.396225929260254</v>
       </c>
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>1.629676262382418E-4</v>
+        <v>1.6292768123093992E-4</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>14</v>
@@ -245,7 +245,7 @@
         <v>13</v>
       </c>
       <c r="H4" t="n" s="2">
-        <v>5.309144020080566</v>
+        <v>5.288824081420898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>